<commit_message>
Json per Euramet funzionante
inizio lavoro sulla guida per Fabio
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
@@ -9971,7 +9971,7 @@
       </c>
       <c r="B63" s="526" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C63" s="52" t="n"/>
@@ -9984,7 +9984,7 @@
       </c>
       <c r="B64" s="54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C64" s="52" t="n"/>
@@ -9997,7 +9997,7 @@
       </c>
       <c r="B65" s="54" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C65" s="52" t="inlineStr">
@@ -10014,7 +10014,7 @@
       </c>
       <c r="B66" s="54" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C66" s="52" t="inlineStr">
@@ -10031,7 +10031,7 @@
       </c>
       <c r="B67" s="54" t="inlineStr">
         <is>
-          <t>tre</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -10053,7 +10053,7 @@
       </c>
       <c r="B68" s="54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C68" s="52" t="inlineStr">
@@ -10070,7 +10070,7 @@
       </c>
       <c r="B69" s="54" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C69" s="52" t="inlineStr">
@@ -10088,7 +10088,7 @@
       </c>
       <c r="B70" s="54" t="inlineStr">
         <is>
-          <t>sei</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C70" s="52" t="inlineStr">

</xml_diff>

<commit_message>
eseguibile creato, ora cerco di migliorare
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
@@ -5108,7 +5108,7 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
     <col width="9" customWidth="1" style="363" min="1" max="1"/>
     <col width="10.33203125" customWidth="1" style="363" min="2" max="2"/>
@@ -5312,16 +5312,16 @@
         <v>837</v>
       </c>
       <c r="E7" s="419" t="n">
-        <v>989</v>
+        <v>0</v>
       </c>
       <c r="F7" s="419" t="n">
-        <v>-0.3</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G7" s="419" t="n">
-        <v>-2.4</v>
+        <v>-1.3734</v>
       </c>
       <c r="H7" s="420" t="n">
-        <v>2.42215</v>
+        <v>0.001</v>
       </c>
       <c r="I7" s="364">
         <f>(H7-$E$5)+$H$2</f>
@@ -5381,16 +5381,16 @@
         <v>837</v>
       </c>
       <c r="E8" s="339" t="n">
-        <v>883</v>
+        <v>0</v>
       </c>
       <c r="F8" s="339" t="n">
-        <v>257</v>
+        <v>-156.5579745837849</v>
       </c>
       <c r="G8" s="339" t="n">
-        <v>-253.9</v>
+        <v>-1.1772</v>
       </c>
       <c r="H8" s="422" t="n">
-        <v>1.90669</v>
+        <v>0.001</v>
       </c>
       <c r="I8" s="365">
         <f>(H8-$E$5)+$H$2</f>
@@ -5446,11 +5446,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D9" s="421" t="n"/>
-      <c r="E9" s="339" t="n"/>
-      <c r="F9" s="339" t="n"/>
-      <c r="G9" s="339" t="n"/>
-      <c r="H9" s="422" t="n"/>
+      <c r="D9" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E9" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="339" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G9" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H9" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I9" s="365">
         <f>(H9-$E$5)+$H$2</f>
         <v/>
@@ -5505,11 +5515,21 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D10" s="421" t="n"/>
-      <c r="E10" s="339" t="n"/>
-      <c r="F10" s="339" t="n"/>
-      <c r="G10" s="339" t="n"/>
-      <c r="H10" s="422" t="n"/>
+      <c r="D10" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E10" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="339" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G10" s="339" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H10" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I10" s="365">
         <f>(H10-$E$5)+$H$2</f>
         <v/>
@@ -5564,11 +5584,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D11" s="421" t="n"/>
-      <c r="E11" s="339" t="n"/>
-      <c r="F11" s="339" t="n"/>
-      <c r="G11" s="339" t="n"/>
-      <c r="H11" s="422" t="n"/>
+      <c r="D11" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E11" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="339" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G11" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H11" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I11" s="365">
         <f>(H11-$E$5)+$H$2</f>
         <v/>
@@ -5623,11 +5653,21 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D12" s="421" t="n"/>
-      <c r="E12" s="339" t="n"/>
-      <c r="F12" s="339" t="n"/>
-      <c r="G12" s="339" t="n"/>
-      <c r="H12" s="422" t="n"/>
+      <c r="D12" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E12" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="339" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G12" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H12" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I12" s="365">
         <f>(H12-$E$5)+$H$2</f>
         <v/>
@@ -5682,11 +5722,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D13" s="423" t="n"/>
-      <c r="E13" s="343" t="n"/>
-      <c r="F13" s="343" t="n"/>
-      <c r="G13" s="343" t="n"/>
-      <c r="H13" s="424" t="n"/>
+      <c r="D13" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E13" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="343" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G13" s="343" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H13" s="424" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I13" s="364">
         <f>(H13-$E$5)+$H$2</f>
         <v/>
@@ -5741,11 +5791,21 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D14" s="425" t="n"/>
-      <c r="E14" s="344" t="n"/>
-      <c r="F14" s="344" t="n"/>
-      <c r="G14" s="344" t="n"/>
-      <c r="H14" s="426" t="n"/>
+      <c r="D14" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E14" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G14" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H14" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I14" s="365">
         <f>(H14-$E$5)+$H$2</f>
         <v/>
@@ -5800,11 +5860,21 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D15" s="425" t="n"/>
-      <c r="E15" s="344" t="n"/>
-      <c r="F15" s="344" t="n"/>
-      <c r="G15" s="344" t="n"/>
-      <c r="H15" s="426" t="n"/>
+      <c r="D15" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E15" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G15" s="344" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H15" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I15" s="365">
         <f>(H15-$E$5)+$H$2</f>
         <v/>
@@ -5859,11 +5929,21 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D16" s="425" t="n"/>
-      <c r="E16" s="344" t="n"/>
-      <c r="F16" s="344" t="n"/>
-      <c r="G16" s="344" t="n"/>
-      <c r="H16" s="426" t="n"/>
+      <c r="D16" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E16" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G16" s="344" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H16" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I16" s="365">
         <f>(H16-$E$5)+$H$2</f>
         <v/>
@@ -5918,11 +5998,21 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D17" s="425" t="n"/>
-      <c r="E17" s="344" t="n"/>
-      <c r="F17" s="344" t="n"/>
-      <c r="G17" s="344" t="n"/>
-      <c r="H17" s="426" t="n"/>
+      <c r="D17" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E17" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G17" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H17" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I17" s="365">
         <f>(H17-$E$5)+$H$2</f>
         <v/>
@@ -5977,11 +6067,21 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D18" s="425" t="n"/>
-      <c r="E18" s="344" t="n"/>
-      <c r="F18" s="344" t="n"/>
-      <c r="G18" s="344" t="n"/>
-      <c r="H18" s="426" t="n"/>
+      <c r="D18" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E18" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G18" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H18" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I18" s="365">
         <f>(H18-$E$5)+$H$2</f>
         <v/>
@@ -6036,11 +6136,21 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D19" s="423" t="n"/>
-      <c r="E19" s="343" t="n"/>
-      <c r="F19" s="343" t="n"/>
-      <c r="G19" s="343" t="n"/>
-      <c r="H19" s="424" t="n"/>
+      <c r="D19" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E19" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="343" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G19" s="343" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H19" s="424" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I19" s="364">
         <f>(H19-$E$5)+$H$2</f>
         <v/>
@@ -6566,11 +6676,21 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D29" s="418" t="n"/>
-      <c r="E29" s="419" t="n"/>
-      <c r="F29" s="419" t="n"/>
-      <c r="G29" s="419" t="n"/>
-      <c r="H29" s="420" t="n"/>
+      <c r="D29" s="418" t="n">
+        <v>837</v>
+      </c>
+      <c r="E29" s="419" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="419" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G29" s="419" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H29" s="420" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I29" s="364">
         <f>(H29-$E$27)+$H$2</f>
         <v/>
@@ -6625,11 +6745,21 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D30" s="421" t="n"/>
-      <c r="E30" s="339" t="n"/>
-      <c r="F30" s="339" t="n"/>
-      <c r="G30" s="339" t="n"/>
-      <c r="H30" s="422" t="n"/>
+      <c r="D30" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E30" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G30" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H30" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I30" s="365">
         <f>(H30-$E$27)+$H$2</f>
         <v/>
@@ -6684,11 +6814,21 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D31" s="421" t="n"/>
-      <c r="E31" s="339" t="n"/>
-      <c r="F31" s="339" t="n"/>
-      <c r="G31" s="339" t="n"/>
-      <c r="H31" s="422" t="n"/>
+      <c r="D31" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E31" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G31" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H31" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I31" s="365">
         <f>(H31-$E$27)+$H$2</f>
         <v/>
@@ -6743,11 +6883,21 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D32" s="421" t="n"/>
-      <c r="E32" s="339" t="n"/>
-      <c r="F32" s="339" t="n"/>
-      <c r="G32" s="339" t="n"/>
-      <c r="H32" s="422" t="n"/>
+      <c r="D32" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E32" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G32" s="339" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H32" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I32" s="365">
         <f>(H32-$E$27)+$H$2</f>
         <v/>
@@ -6802,11 +6952,21 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D33" s="421" t="n"/>
-      <c r="E33" s="339" t="n"/>
-      <c r="F33" s="339" t="n"/>
-      <c r="G33" s="339" t="n"/>
-      <c r="H33" s="422" t="n"/>
+      <c r="D33" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E33" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G33" s="339" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H33" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I33" s="365">
         <f>(H33-$E$27)+$H$2</f>
         <v/>
@@ -6861,11 +7021,21 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D34" s="421" t="n"/>
-      <c r="E34" s="339" t="n"/>
-      <c r="F34" s="339" t="n"/>
-      <c r="G34" s="339" t="n"/>
-      <c r="H34" s="422" t="n"/>
+      <c r="D34" s="421" t="n">
+        <v>837</v>
+      </c>
+      <c r="E34" s="339" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="339" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G34" s="339" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H34" s="422" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I34" s="365">
         <f>(H34-$E$27)+$H$2</f>
         <v/>
@@ -6920,11 +7090,21 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D35" s="423" t="n"/>
-      <c r="E35" s="343" t="n"/>
-      <c r="F35" s="343" t="n"/>
-      <c r="G35" s="343" t="n"/>
-      <c r="H35" s="424" t="n"/>
+      <c r="D35" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E35" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="343" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G35" s="343" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H35" s="424" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I35" s="364">
         <f>(H35-$E$27)+$H$2</f>
         <v/>
@@ -6979,11 +7159,21 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D36" s="425" t="n"/>
-      <c r="E36" s="344" t="n"/>
-      <c r="F36" s="344" t="n"/>
-      <c r="G36" s="344" t="n"/>
-      <c r="H36" s="426" t="n"/>
+      <c r="D36" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E36" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G36" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H36" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I36" s="365">
         <f>(H36-$E$27)+$H$2</f>
         <v/>
@@ -7038,11 +7228,21 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D37" s="425" t="n"/>
-      <c r="E37" s="344" t="n"/>
-      <c r="F37" s="344" t="n"/>
-      <c r="G37" s="344" t="n"/>
-      <c r="H37" s="426" t="n"/>
+      <c r="D37" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E37" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G37" s="344" t="n">
+        <v>-1.3734</v>
+      </c>
+      <c r="H37" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I37" s="365">
         <f>(H37-$E$27)+$H$2</f>
         <v/>
@@ -7097,11 +7297,21 @@
         <f>SetPnt_P_3</f>
         <v/>
       </c>
-      <c r="D38" s="425" t="n"/>
-      <c r="E38" s="344" t="n"/>
-      <c r="F38" s="344" t="n"/>
-      <c r="G38" s="344" t="n"/>
-      <c r="H38" s="426" t="n"/>
+      <c r="D38" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E38" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="344" t="n">
+        <v>-156.5579745837849</v>
+      </c>
+      <c r="G38" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H38" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I38" s="365">
         <f>(H38-$E$27)+$H$2</f>
         <v/>
@@ -7156,11 +7366,21 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D39" s="425" t="n"/>
-      <c r="E39" s="344" t="n"/>
-      <c r="F39" s="344" t="n"/>
-      <c r="G39" s="344" t="n"/>
-      <c r="H39" s="426" t="n"/>
+      <c r="D39" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E39" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G39" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H39" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I39" s="365">
         <f>(H39-$E$27)+$H$2</f>
         <v/>
@@ -7215,11 +7435,21 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D40" s="425" t="n"/>
-      <c r="E40" s="344" t="n"/>
-      <c r="F40" s="344" t="n"/>
-      <c r="G40" s="344" t="n"/>
-      <c r="H40" s="426" t="n"/>
+      <c r="D40" s="425" t="n">
+        <v>837</v>
+      </c>
+      <c r="E40" s="344" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="344" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G40" s="344" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H40" s="426" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I40" s="365">
         <f>(H40-$E$27)+$H$2</f>
         <v/>
@@ -7274,11 +7504,21 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D41" s="423" t="n"/>
-      <c r="E41" s="343" t="n"/>
-      <c r="F41" s="343" t="n"/>
-      <c r="G41" s="343" t="n"/>
-      <c r="H41" s="424" t="n"/>
+      <c r="D41" s="423" t="n">
+        <v>837</v>
+      </c>
+      <c r="E41" s="343" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="343" t="n">
+        <v>-157.0411782090434</v>
+      </c>
+      <c r="G41" s="343" t="n">
+        <v>-1.1772</v>
+      </c>
+      <c r="H41" s="424" t="n">
+        <v>0.001</v>
+      </c>
       <c r="I41" s="364">
         <f>(H41-$E$27)+$H$2</f>
         <v/>
@@ -8619,11 +8859,11 @@
     <mergeCell ref="B74:B75"/>
     <mergeCell ref="B50:H51"/>
     <mergeCell ref="B60:B61"/>
-    <mergeCell ref="G60:H60"/>
     <mergeCell ref="A74:A85"/>
     <mergeCell ref="C74:D74"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="E60:F60"/>
     <mergeCell ref="A60:A71"/>
-    <mergeCell ref="E60:F60"/>
     <mergeCell ref="E74:F74"/>
     <mergeCell ref="G74:H74"/>
     <mergeCell ref="K50:Q51"/>
@@ -8701,7 +8941,7 @@
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col width="25.88671875" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
@@ -9997,7 +10237,7 @@
       </c>
       <c r="B65" s="54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>w</t>
         </is>
       </c>
       <c r="C65" s="52" t="inlineStr">
@@ -10014,7 +10254,7 @@
       </c>
       <c r="B66" s="54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ww</t>
         </is>
       </c>
       <c r="C66" s="52" t="inlineStr">
@@ -10031,7 +10271,7 @@
       </c>
       <c r="B67" s="54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>w</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -10053,7 +10293,7 @@
       </c>
       <c r="B68" s="54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>wwww</t>
         </is>
       </c>
       <c r="C68" s="52" t="inlineStr">
@@ -10070,7 +10310,7 @@
       </c>
       <c r="B69" s="54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>twwww</t>
         </is>
       </c>
       <c r="C69" s="52" t="inlineStr">
@@ -10292,7 +10532,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col width="15.5546875" customWidth="1" min="1" max="1"/>
     <col width="19.6640625" customWidth="1" min="2" max="2"/>
@@ -16515,7 +16755,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col width="14.33203125" customWidth="1" min="1" max="1"/>
     <col width="19.6640625" customWidth="1" min="2" max="2"/>
@@ -22712,7 +22952,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="9" customWidth="1" min="2" max="2"/>
     <col width="13.5546875" customWidth="1" min="3" max="3"/>
@@ -23877,7 +24117,7 @@
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="3" customWidth="1" min="1" max="1"/>
     <col width="3.5546875" customWidth="1" min="2" max="2"/>
@@ -25385,8 +25625,8 @@
     <mergeCell ref="C7:L7"/>
     <mergeCell ref="F10:M10"/>
     <mergeCell ref="F16:M16"/>
+    <mergeCell ref="L102:L103"/>
     <mergeCell ref="G70:H70"/>
-    <mergeCell ref="L102:L103"/>
     <mergeCell ref="G97:H97"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="I70:J70"/>

</xml_diff>

<commit_message>
pausa lavoro su eseguibile
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
@@ -5108,7 +5108,7 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
     <col width="9" customWidth="1" style="363" min="1" max="1"/>
     <col width="10.33203125" customWidth="1" style="363" min="2" max="2"/>
@@ -5312,16 +5312,16 @@
         <v>837</v>
       </c>
       <c r="E7" s="419" t="n">
-        <v>0</v>
+        <v>989</v>
       </c>
       <c r="F7" s="419" t="n">
-        <v>-157.0411782090434</v>
+        <v>-0.3</v>
       </c>
       <c r="G7" s="419" t="n">
-        <v>-1.3734</v>
+        <v>-2.4</v>
       </c>
       <c r="H7" s="420" t="n">
-        <v>0.001</v>
+        <v>2.42215</v>
       </c>
       <c r="I7" s="364">
         <f>(H7-$E$5)+$H$2</f>
@@ -5381,16 +5381,16 @@
         <v>837</v>
       </c>
       <c r="E8" s="339" t="n">
-        <v>0</v>
+        <v>883</v>
       </c>
       <c r="F8" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>257</v>
       </c>
       <c r="G8" s="339" t="n">
-        <v>-1.1772</v>
+        <v>-253.9</v>
       </c>
       <c r="H8" s="422" t="n">
-        <v>0.001</v>
+        <v>1.90669</v>
       </c>
       <c r="I8" s="365">
         <f>(H8-$E$5)+$H$2</f>
@@ -5446,21 +5446,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D9" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E9" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G9" s="339" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H9" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D9" s="421" t="n"/>
+      <c r="E9" s="339" t="n"/>
+      <c r="F9" s="339" t="n"/>
+      <c r="G9" s="339" t="n"/>
+      <c r="H9" s="422" t="n"/>
       <c r="I9" s="365">
         <f>(H9-$E$5)+$H$2</f>
         <v/>
@@ -5515,21 +5505,11 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D10" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E10" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G10" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H10" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D10" s="421" t="n"/>
+      <c r="E10" s="339" t="n"/>
+      <c r="F10" s="339" t="n"/>
+      <c r="G10" s="339" t="n"/>
+      <c r="H10" s="422" t="n"/>
       <c r="I10" s="365">
         <f>(H10-$E$5)+$H$2</f>
         <v/>
@@ -5584,21 +5564,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D11" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E11" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G11" s="339" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H11" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D11" s="421" t="n"/>
+      <c r="E11" s="339" t="n"/>
+      <c r="F11" s="339" t="n"/>
+      <c r="G11" s="339" t="n"/>
+      <c r="H11" s="422" t="n"/>
       <c r="I11" s="365">
         <f>(H11-$E$5)+$H$2</f>
         <v/>
@@ -5653,21 +5623,11 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D12" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E12" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G12" s="339" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H12" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D12" s="421" t="n"/>
+      <c r="E12" s="339" t="n"/>
+      <c r="F12" s="339" t="n"/>
+      <c r="G12" s="339" t="n"/>
+      <c r="H12" s="422" t="n"/>
       <c r="I12" s="365">
         <f>(H12-$E$5)+$H$2</f>
         <v/>
@@ -5722,21 +5682,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D13" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E13" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G13" s="343" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H13" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D13" s="423" t="n"/>
+      <c r="E13" s="343" t="n"/>
+      <c r="F13" s="343" t="n"/>
+      <c r="G13" s="343" t="n"/>
+      <c r="H13" s="424" t="n"/>
       <c r="I13" s="364">
         <f>(H13-$E$5)+$H$2</f>
         <v/>
@@ -5791,21 +5741,11 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D14" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E14" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G14" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H14" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D14" s="425" t="n"/>
+      <c r="E14" s="344" t="n"/>
+      <c r="F14" s="344" t="n"/>
+      <c r="G14" s="344" t="n"/>
+      <c r="H14" s="426" t="n"/>
       <c r="I14" s="365">
         <f>(H14-$E$5)+$H$2</f>
         <v/>
@@ -5860,21 +5800,11 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D15" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E15" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G15" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H15" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D15" s="425" t="n"/>
+      <c r="E15" s="344" t="n"/>
+      <c r="F15" s="344" t="n"/>
+      <c r="G15" s="344" t="n"/>
+      <c r="H15" s="426" t="n"/>
       <c r="I15" s="365">
         <f>(H15-$E$5)+$H$2</f>
         <v/>
@@ -5929,21 +5859,11 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D16" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E16" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G16" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H16" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D16" s="425" t="n"/>
+      <c r="E16" s="344" t="n"/>
+      <c r="F16" s="344" t="n"/>
+      <c r="G16" s="344" t="n"/>
+      <c r="H16" s="426" t="n"/>
       <c r="I16" s="365">
         <f>(H16-$E$5)+$H$2</f>
         <v/>
@@ -5998,21 +5918,11 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D17" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E17" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G17" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H17" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D17" s="425" t="n"/>
+      <c r="E17" s="344" t="n"/>
+      <c r="F17" s="344" t="n"/>
+      <c r="G17" s="344" t="n"/>
+      <c r="H17" s="426" t="n"/>
       <c r="I17" s="365">
         <f>(H17-$E$5)+$H$2</f>
         <v/>
@@ -6067,21 +5977,11 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D18" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E18" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G18" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H18" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D18" s="425" t="n"/>
+      <c r="E18" s="344" t="n"/>
+      <c r="F18" s="344" t="n"/>
+      <c r="G18" s="344" t="n"/>
+      <c r="H18" s="426" t="n"/>
       <c r="I18" s="365">
         <f>(H18-$E$5)+$H$2</f>
         <v/>
@@ -6136,21 +6036,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D19" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E19" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G19" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H19" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D19" s="423" t="n"/>
+      <c r="E19" s="343" t="n"/>
+      <c r="F19" s="343" t="n"/>
+      <c r="G19" s="343" t="n"/>
+      <c r="H19" s="424" t="n"/>
       <c r="I19" s="364">
         <f>(H19-$E$5)+$H$2</f>
         <v/>
@@ -6676,21 +6566,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D29" s="418" t="n">
-        <v>837</v>
-      </c>
-      <c r="E29" s="419" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="419" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G29" s="419" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H29" s="420" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D29" s="418" t="n"/>
+      <c r="E29" s="419" t="n"/>
+      <c r="F29" s="419" t="n"/>
+      <c r="G29" s="419" t="n"/>
+      <c r="H29" s="420" t="n"/>
       <c r="I29" s="364">
         <f>(H29-$E$27)+$H$2</f>
         <v/>
@@ -6745,21 +6625,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D30" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E30" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G30" s="339" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H30" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D30" s="421" t="n"/>
+      <c r="E30" s="339" t="n"/>
+      <c r="F30" s="339" t="n"/>
+      <c r="G30" s="339" t="n"/>
+      <c r="H30" s="422" t="n"/>
       <c r="I30" s="365">
         <f>(H30-$E$27)+$H$2</f>
         <v/>
@@ -6814,21 +6684,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D31" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E31" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G31" s="339" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H31" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D31" s="421" t="n"/>
+      <c r="E31" s="339" t="n"/>
+      <c r="F31" s="339" t="n"/>
+      <c r="G31" s="339" t="n"/>
+      <c r="H31" s="422" t="n"/>
       <c r="I31" s="365">
         <f>(H31-$E$27)+$H$2</f>
         <v/>
@@ -6883,21 +6743,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D32" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E32" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G32" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H32" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D32" s="421" t="n"/>
+      <c r="E32" s="339" t="n"/>
+      <c r="F32" s="339" t="n"/>
+      <c r="G32" s="339" t="n"/>
+      <c r="H32" s="422" t="n"/>
       <c r="I32" s="365">
         <f>(H32-$E$27)+$H$2</f>
         <v/>
@@ -6952,21 +6802,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D33" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E33" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G33" s="339" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H33" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D33" s="421" t="n"/>
+      <c r="E33" s="339" t="n"/>
+      <c r="F33" s="339" t="n"/>
+      <c r="G33" s="339" t="n"/>
+      <c r="H33" s="422" t="n"/>
       <c r="I33" s="365">
         <f>(H33-$E$27)+$H$2</f>
         <v/>
@@ -7021,21 +6861,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D34" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E34" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G34" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H34" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D34" s="421" t="n"/>
+      <c r="E34" s="339" t="n"/>
+      <c r="F34" s="339" t="n"/>
+      <c r="G34" s="339" t="n"/>
+      <c r="H34" s="422" t="n"/>
       <c r="I34" s="365">
         <f>(H34-$E$27)+$H$2</f>
         <v/>
@@ -7090,21 +6920,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D35" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E35" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G35" s="343" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H35" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D35" s="423" t="n"/>
+      <c r="E35" s="343" t="n"/>
+      <c r="F35" s="343" t="n"/>
+      <c r="G35" s="343" t="n"/>
+      <c r="H35" s="424" t="n"/>
       <c r="I35" s="364">
         <f>(H35-$E$27)+$H$2</f>
         <v/>
@@ -7159,21 +6979,11 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D36" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E36" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G36" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H36" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D36" s="425" t="n"/>
+      <c r="E36" s="344" t="n"/>
+      <c r="F36" s="344" t="n"/>
+      <c r="G36" s="344" t="n"/>
+      <c r="H36" s="426" t="n"/>
       <c r="I36" s="365">
         <f>(H36-$E$27)+$H$2</f>
         <v/>
@@ -7228,21 +7038,11 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D37" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E37" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G37" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H37" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D37" s="425" t="n"/>
+      <c r="E37" s="344" t="n"/>
+      <c r="F37" s="344" t="n"/>
+      <c r="G37" s="344" t="n"/>
+      <c r="H37" s="426" t="n"/>
       <c r="I37" s="365">
         <f>(H37-$E$27)+$H$2</f>
         <v/>
@@ -7297,21 +7097,11 @@
         <f>SetPnt_P_3</f>
         <v/>
       </c>
-      <c r="D38" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E38" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G38" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H38" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D38" s="425" t="n"/>
+      <c r="E38" s="344" t="n"/>
+      <c r="F38" s="344" t="n"/>
+      <c r="G38" s="344" t="n"/>
+      <c r="H38" s="426" t="n"/>
       <c r="I38" s="365">
         <f>(H38-$E$27)+$H$2</f>
         <v/>
@@ -7366,21 +7156,11 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D39" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E39" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G39" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H39" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D39" s="425" t="n"/>
+      <c r="E39" s="344" t="n"/>
+      <c r="F39" s="344" t="n"/>
+      <c r="G39" s="344" t="n"/>
+      <c r="H39" s="426" t="n"/>
       <c r="I39" s="365">
         <f>(H39-$E$27)+$H$2</f>
         <v/>
@@ -7435,21 +7215,11 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D40" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E40" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G40" s="344" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H40" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D40" s="425" t="n"/>
+      <c r="E40" s="344" t="n"/>
+      <c r="F40" s="344" t="n"/>
+      <c r="G40" s="344" t="n"/>
+      <c r="H40" s="426" t="n"/>
       <c r="I40" s="365">
         <f>(H40-$E$27)+$H$2</f>
         <v/>
@@ -7504,21 +7274,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D41" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E41" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G41" s="343" t="n">
-        <v>-1.1772</v>
-      </c>
-      <c r="H41" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D41" s="423" t="n"/>
+      <c r="E41" s="343" t="n"/>
+      <c r="F41" s="343" t="n"/>
+      <c r="G41" s="343" t="n"/>
+      <c r="H41" s="424" t="n"/>
       <c r="I41" s="364">
         <f>(H41-$E$27)+$H$2</f>
         <v/>
@@ -8859,11 +8619,11 @@
     <mergeCell ref="B74:B75"/>
     <mergeCell ref="B50:H51"/>
     <mergeCell ref="B60:B61"/>
+    <mergeCell ref="G60:H60"/>
     <mergeCell ref="A74:A85"/>
     <mergeCell ref="C74:D74"/>
-    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="A60:A71"/>
     <mergeCell ref="E60:F60"/>
-    <mergeCell ref="A60:A71"/>
     <mergeCell ref="E74:F74"/>
     <mergeCell ref="G74:H74"/>
     <mergeCell ref="K50:Q51"/>
@@ -8941,7 +8701,7 @@
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="25.88671875" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
@@ -10237,7 +9997,7 @@
       </c>
       <c r="B65" s="54" t="inlineStr">
         <is>
-          <t>w</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C65" s="52" t="inlineStr">
@@ -10254,7 +10014,7 @@
       </c>
       <c r="B66" s="54" t="inlineStr">
         <is>
-          <t>ww</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C66" s="52" t="inlineStr">
@@ -10271,7 +10031,7 @@
       </c>
       <c r="B67" s="54" t="inlineStr">
         <is>
-          <t>w</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -10293,7 +10053,7 @@
       </c>
       <c r="B68" s="54" t="inlineStr">
         <is>
-          <t>wwww</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C68" s="52" t="inlineStr">
@@ -10310,7 +10070,7 @@
       </c>
       <c r="B69" s="54" t="inlineStr">
         <is>
-          <t>twwww</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C69" s="52" t="inlineStr">
@@ -10532,7 +10292,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="15.5546875" customWidth="1" min="1" max="1"/>
     <col width="19.6640625" customWidth="1" min="2" max="2"/>
@@ -16755,7 +16515,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="14.33203125" customWidth="1" min="1" max="1"/>
     <col width="19.6640625" customWidth="1" min="2" max="2"/>
@@ -22952,7 +22712,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col width="9" customWidth="1" min="2" max="2"/>
     <col width="13.5546875" customWidth="1" min="3" max="3"/>
@@ -24117,7 +23877,7 @@
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col width="3" customWidth="1" min="1" max="1"/>
     <col width="3.5546875" customWidth="1" min="2" max="2"/>
@@ -25625,8 +25385,8 @@
     <mergeCell ref="C7:L7"/>
     <mergeCell ref="F10:M10"/>
     <mergeCell ref="F16:M16"/>
+    <mergeCell ref="G70:H70"/>
     <mergeCell ref="L102:L103"/>
-    <mergeCell ref="G70:H70"/>
     <mergeCell ref="G97:H97"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="I70:J70"/>

</xml_diff>

<commit_message>
inserimento finestre di errore
per le connessioni con le schede
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
@@ -5312,13 +5312,13 @@
         <v>837</v>
       </c>
       <c r="E7" s="419" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F7" s="419" t="n">
         <v>-157.0411782090434</v>
       </c>
       <c r="G7" s="419" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H7" s="420" t="n">
         <v>0.001</v>
@@ -5377,21 +5377,11 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D8" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E8" s="339" t="n">
-        <v>22</v>
-      </c>
-      <c r="F8" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G8" s="339" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H8" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D8" s="421" t="n"/>
+      <c r="E8" s="339" t="n"/>
+      <c r="F8" s="339" t="n"/>
+      <c r="G8" s="339" t="n"/>
+      <c r="H8" s="422" t="n"/>
       <c r="I8" s="365">
         <f>(H8-$E$5)+$H$2</f>
         <v/>
@@ -5446,21 +5436,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D9" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E9" s="339" t="n">
-        <v>33</v>
-      </c>
-      <c r="F9" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G9" s="339" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H9" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D9" s="421" t="n"/>
+      <c r="E9" s="339" t="n"/>
+      <c r="F9" s="339" t="n"/>
+      <c r="G9" s="339" t="n"/>
+      <c r="H9" s="422" t="n"/>
       <c r="I9" s="365">
         <f>(H9-$E$5)+$H$2</f>
         <v/>
@@ -5515,21 +5495,11 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D10" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E10" s="339" t="n">
-        <v>44</v>
-      </c>
-      <c r="F10" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G10" s="339" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H10" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D10" s="421" t="n"/>
+      <c r="E10" s="339" t="n"/>
+      <c r="F10" s="339" t="n"/>
+      <c r="G10" s="339" t="n"/>
+      <c r="H10" s="422" t="n"/>
       <c r="I10" s="365">
         <f>(H10-$E$5)+$H$2</f>
         <v/>
@@ -5584,21 +5554,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D11" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E11" s="339" t="n">
-        <v>55</v>
-      </c>
-      <c r="F11" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G11" s="339" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H11" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D11" s="421" t="n"/>
+      <c r="E11" s="339" t="n"/>
+      <c r="F11" s="339" t="n"/>
+      <c r="G11" s="339" t="n"/>
+      <c r="H11" s="422" t="n"/>
       <c r="I11" s="365">
         <f>(H11-$E$5)+$H$2</f>
         <v/>
@@ -5653,21 +5613,11 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D12" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E12" s="339" t="n">
-        <v>66</v>
-      </c>
-      <c r="F12" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G12" s="339" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H12" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D12" s="421" t="n"/>
+      <c r="E12" s="339" t="n"/>
+      <c r="F12" s="339" t="n"/>
+      <c r="G12" s="339" t="n"/>
+      <c r="H12" s="422" t="n"/>
       <c r="I12" s="365">
         <f>(H12-$E$5)+$H$2</f>
         <v/>
@@ -5722,21 +5672,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D13" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E13" s="343" t="n">
-        <v>77</v>
-      </c>
-      <c r="F13" s="343" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G13" s="343" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H13" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D13" s="423" t="n"/>
+      <c r="E13" s="343" t="n"/>
+      <c r="F13" s="343" t="n"/>
+      <c r="G13" s="343" t="n"/>
+      <c r="H13" s="424" t="n"/>
       <c r="I13" s="364">
         <f>(H13-$E$5)+$H$2</f>
         <v/>
@@ -5791,21 +5731,11 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D14" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E14" s="344" t="n">
-        <v>88</v>
-      </c>
-      <c r="F14" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G14" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H14" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D14" s="425" t="n"/>
+      <c r="E14" s="344" t="n"/>
+      <c r="F14" s="344" t="n"/>
+      <c r="G14" s="344" t="n"/>
+      <c r="H14" s="426" t="n"/>
       <c r="I14" s="365">
         <f>(H14-$E$5)+$H$2</f>
         <v/>
@@ -5860,21 +5790,11 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D15" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E15" s="344" t="n">
-        <v>99</v>
-      </c>
-      <c r="F15" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G15" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H15" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D15" s="425" t="n"/>
+      <c r="E15" s="344" t="n"/>
+      <c r="F15" s="344" t="n"/>
+      <c r="G15" s="344" t="n"/>
+      <c r="H15" s="426" t="n"/>
       <c r="I15" s="365">
         <f>(H15-$E$5)+$H$2</f>
         <v/>
@@ -5929,21 +5849,11 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D16" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E16" s="344" t="n">
-        <v>111</v>
-      </c>
-      <c r="F16" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G16" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H16" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D16" s="425" t="n"/>
+      <c r="E16" s="344" t="n"/>
+      <c r="F16" s="344" t="n"/>
+      <c r="G16" s="344" t="n"/>
+      <c r="H16" s="426" t="n"/>
       <c r="I16" s="365">
         <f>(H16-$E$5)+$H$2</f>
         <v/>
@@ -5998,21 +5908,11 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D17" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E17" s="344" t="n">
-        <v>222</v>
-      </c>
-      <c r="F17" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G17" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H17" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D17" s="425" t="n"/>
+      <c r="E17" s="344" t="n"/>
+      <c r="F17" s="344" t="n"/>
+      <c r="G17" s="344" t="n"/>
+      <c r="H17" s="426" t="n"/>
       <c r="I17" s="365">
         <f>(H17-$E$5)+$H$2</f>
         <v/>
@@ -6067,21 +5967,11 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D18" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E18" s="344" t="n">
-        <v>333</v>
-      </c>
-      <c r="F18" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G18" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H18" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D18" s="425" t="n"/>
+      <c r="E18" s="344" t="n"/>
+      <c r="F18" s="344" t="n"/>
+      <c r="G18" s="344" t="n"/>
+      <c r="H18" s="426" t="n"/>
       <c r="I18" s="365">
         <f>(H18-$E$5)+$H$2</f>
         <v/>
@@ -6136,21 +6026,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D19" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E19" s="343" t="n">
-        <v>444</v>
-      </c>
-      <c r="F19" s="343" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G19" s="343" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H19" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D19" s="423" t="n"/>
+      <c r="E19" s="343" t="n"/>
+      <c r="F19" s="343" t="n"/>
+      <c r="G19" s="343" t="n"/>
+      <c r="H19" s="424" t="n"/>
       <c r="I19" s="364">
         <f>(H19-$E$5)+$H$2</f>
         <v/>
@@ -6205,21 +6085,11 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D20" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E20" s="344" t="n">
-        <v>555</v>
-      </c>
-      <c r="F20" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G20" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H20" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D20" s="425" t="n"/>
+      <c r="E20" s="344" t="n"/>
+      <c r="F20" s="344" t="n"/>
+      <c r="G20" s="344" t="n"/>
+      <c r="H20" s="426" t="n"/>
       <c r="I20" s="365">
         <f>(H20-$E$5)+$H$2</f>
         <v/>
@@ -6274,21 +6144,11 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D21" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E21" s="344" t="n">
-        <v>666</v>
-      </c>
-      <c r="F21" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G21" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H21" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D21" s="425" t="n"/>
+      <c r="E21" s="344" t="n"/>
+      <c r="F21" s="344" t="n"/>
+      <c r="G21" s="344" t="n"/>
+      <c r="H21" s="426" t="n"/>
       <c r="I21" s="365">
         <f>(H21-$E$5)+$H$2</f>
         <v/>
@@ -6343,21 +6203,11 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D22" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E22" s="344" t="n">
-        <v>777</v>
-      </c>
-      <c r="F22" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G22" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H22" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D22" s="425" t="n"/>
+      <c r="E22" s="344" t="n"/>
+      <c r="F22" s="344" t="n"/>
+      <c r="G22" s="344" t="n"/>
+      <c r="H22" s="426" t="n"/>
       <c r="I22" s="365">
         <f>(H22-$E$5)+$H$2</f>
         <v/>
@@ -6412,21 +6262,11 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D23" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E23" s="344" t="n">
-        <v>888</v>
-      </c>
-      <c r="F23" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G23" s="344" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H23" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D23" s="425" t="n"/>
+      <c r="E23" s="344" t="n"/>
+      <c r="F23" s="344" t="n"/>
+      <c r="G23" s="344" t="n"/>
+      <c r="H23" s="426" t="n"/>
       <c r="I23" s="365">
         <f>(H23-$E$5)+$H$2</f>
         <v/>
@@ -6481,21 +6321,11 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D24" s="427" t="n">
-        <v>837</v>
-      </c>
-      <c r="E24" s="348" t="n">
-        <v>999</v>
-      </c>
-      <c r="F24" s="348" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G24" s="348" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H24" s="428" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D24" s="427" t="n"/>
+      <c r="E24" s="348" t="n"/>
+      <c r="F24" s="348" t="n"/>
+      <c r="G24" s="348" t="n"/>
+      <c r="H24" s="428" t="n"/>
       <c r="I24" s="366">
         <f>(H24-$E$5)+$H$2</f>
         <v/>
@@ -6550,21 +6380,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D25" s="429" t="n">
-        <v>837</v>
-      </c>
-      <c r="E25" s="430" t="n">
-        <v>1111</v>
-      </c>
-      <c r="F25" s="430" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G25" s="430" t="n">
-        <v>-1.5696</v>
-      </c>
-      <c r="H25" s="431" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D25" s="429" t="n"/>
+      <c r="E25" s="430" t="n"/>
+      <c r="F25" s="430" t="n"/>
+      <c r="G25" s="430" t="n"/>
+      <c r="H25" s="431" t="n"/>
       <c r="I25" s="366">
         <f>(H25-$E$5)+$H$2</f>
         <v/>
@@ -6740,13 +6560,13 @@
         <v>837</v>
       </c>
       <c r="E29" s="419" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="419" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G29" s="419" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H29" s="420" t="n">
         <v>0.001</v>
@@ -6809,13 +6629,13 @@
         <v>837</v>
       </c>
       <c r="E30" s="339" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F30" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G30" s="339" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H30" s="422" t="n">
         <v>0.001</v>
@@ -6878,13 +6698,13 @@
         <v>837</v>
       </c>
       <c r="E31" s="339" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F31" s="339" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G31" s="339" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H31" s="422" t="n">
         <v>0.001</v>
@@ -6947,13 +6767,13 @@
         <v>837</v>
       </c>
       <c r="E32" s="339" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F32" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G32" s="339" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H32" s="422" t="n">
         <v>0.001</v>
@@ -7016,13 +6836,13 @@
         <v>837</v>
       </c>
       <c r="E33" s="339" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F33" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G33" s="339" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H33" s="422" t="n">
         <v>0.001</v>
@@ -7085,13 +6905,13 @@
         <v>837</v>
       </c>
       <c r="E34" s="339" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F34" s="339" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G34" s="339" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H34" s="422" t="n">
         <v>0.001</v>
@@ -7154,13 +6974,13 @@
         <v>837</v>
       </c>
       <c r="E35" s="343" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F35" s="343" t="n">
         <v>-157.0411782090434</v>
       </c>
       <c r="G35" s="343" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H35" s="424" t="n">
         <v>0.001</v>
@@ -7223,13 +7043,13 @@
         <v>837</v>
       </c>
       <c r="E36" s="344" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F36" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G36" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H36" s="426" t="n">
         <v>0.001</v>
@@ -7292,13 +7112,13 @@
         <v>837</v>
       </c>
       <c r="E37" s="344" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F37" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G37" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H37" s="426" t="n">
         <v>0.001</v>
@@ -7361,13 +7181,13 @@
         <v>837</v>
       </c>
       <c r="E38" s="344" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F38" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G38" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H38" s="426" t="n">
         <v>0.001</v>
@@ -7430,13 +7250,13 @@
         <v>837</v>
       </c>
       <c r="E39" s="344" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F39" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G39" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H39" s="426" t="n">
         <v>0.001</v>
@@ -7499,13 +7319,13 @@
         <v>837</v>
       </c>
       <c r="E40" s="344" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F40" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G40" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H40" s="426" t="n">
         <v>0.001</v>
@@ -7568,13 +7388,13 @@
         <v>837</v>
       </c>
       <c r="E41" s="343" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F41" s="343" t="n">
         <v>-157.0411782090434</v>
       </c>
       <c r="G41" s="343" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H41" s="424" t="n">
         <v>0.001</v>
@@ -7637,13 +7457,13 @@
         <v>837</v>
       </c>
       <c r="E42" s="344" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F42" s="344" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G42" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H42" s="426" t="n">
         <v>0.001</v>
@@ -7706,13 +7526,13 @@
         <v>837</v>
       </c>
       <c r="E43" s="344" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F43" s="344" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G43" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H43" s="426" t="n">
         <v>0.001</v>
@@ -7775,13 +7595,13 @@
         <v>837</v>
       </c>
       <c r="E44" s="344" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F44" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G44" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H44" s="426" t="n">
         <v>0.001</v>
@@ -7844,13 +7664,13 @@
         <v>837</v>
       </c>
       <c r="E45" s="344" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F45" s="344" t="n">
-        <v>-156.5579745837849</v>
+        <v>-157.0411782090434</v>
       </c>
       <c r="G45" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H45" s="426" t="n">
         <v>0.001</v>
@@ -7913,13 +7733,13 @@
         <v>837</v>
       </c>
       <c r="E46" s="344" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F46" s="344" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G46" s="344" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H46" s="426" t="n">
         <v>0.001</v>
@@ -7982,13 +7802,13 @@
         <v>837</v>
       </c>
       <c r="E47" s="430" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F47" s="430" t="n">
         <v>-156.5579745837849</v>
       </c>
       <c r="G47" s="430" t="n">
-        <v>-1.5696</v>
+        <v>-1.3734</v>
       </c>
       <c r="H47" s="431" t="n">
         <v>0.001</v>

</xml_diff>

<commit_message>
sistemati bug per grafica
e inserito label del prossimo step
</commit_message>
<xml_diff>
--- a/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
+++ b/python/Codice_Progetto/Certificati_Euramet_Completi/Default.xlsx
@@ -5108,7 +5108,7 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
     <col width="9" customWidth="1" style="363" min="1" max="1"/>
     <col width="10.33203125" customWidth="1" style="363" min="2" max="2"/>
@@ -5308,21 +5308,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D7" s="418" t="n">
-        <v>837</v>
-      </c>
-      <c r="E7" s="419" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="419" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G7" s="419" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H7" s="420" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D7" s="418" t="n"/>
+      <c r="E7" s="419" t="n"/>
+      <c r="F7" s="419" t="n"/>
+      <c r="G7" s="419" t="n"/>
+      <c r="H7" s="420" t="n"/>
       <c r="I7" s="364">
         <f>(H7-$E$5)+$H$2</f>
         <v/>
@@ -6556,21 +6546,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D29" s="418" t="n">
-        <v>837</v>
-      </c>
-      <c r="E29" s="419" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="419" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G29" s="419" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H29" s="420" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D29" s="418" t="n"/>
+      <c r="E29" s="419" t="n"/>
+      <c r="F29" s="419" t="n"/>
+      <c r="G29" s="419" t="n"/>
+      <c r="H29" s="420" t="n"/>
       <c r="I29" s="364">
         <f>(H29-$E$27)+$H$2</f>
         <v/>
@@ -6625,21 +6605,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D30" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E30" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G30" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H30" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D30" s="421" t="n"/>
+      <c r="E30" s="339" t="n"/>
+      <c r="F30" s="339" t="n"/>
+      <c r="G30" s="339" t="n"/>
+      <c r="H30" s="422" t="n"/>
       <c r="I30" s="365">
         <f>(H30-$E$27)+$H$2</f>
         <v/>
@@ -6694,21 +6664,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D31" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E31" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G31" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H31" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D31" s="421" t="n"/>
+      <c r="E31" s="339" t="n"/>
+      <c r="F31" s="339" t="n"/>
+      <c r="G31" s="339" t="n"/>
+      <c r="H31" s="422" t="n"/>
       <c r="I31" s="365">
         <f>(H31-$E$27)+$H$2</f>
         <v/>
@@ -6763,21 +6723,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D32" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E32" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G32" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H32" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D32" s="421" t="n"/>
+      <c r="E32" s="339" t="n"/>
+      <c r="F32" s="339" t="n"/>
+      <c r="G32" s="339" t="n"/>
+      <c r="H32" s="422" t="n"/>
       <c r="I32" s="365">
         <f>(H32-$E$27)+$H$2</f>
         <v/>
@@ -6832,21 +6782,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D33" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E33" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G33" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H33" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D33" s="421" t="n"/>
+      <c r="E33" s="339" t="n"/>
+      <c r="F33" s="339" t="n"/>
+      <c r="G33" s="339" t="n"/>
+      <c r="H33" s="422" t="n"/>
       <c r="I33" s="365">
         <f>(H33-$E$27)+$H$2</f>
         <v/>
@@ -6901,21 +6841,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D34" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E34" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G34" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H34" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D34" s="421" t="n"/>
+      <c r="E34" s="339" t="n"/>
+      <c r="F34" s="339" t="n"/>
+      <c r="G34" s="339" t="n"/>
+      <c r="H34" s="422" t="n"/>
       <c r="I34" s="365">
         <f>(H34-$E$27)+$H$2</f>
         <v/>
@@ -6970,21 +6900,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D35" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E35" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G35" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H35" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D35" s="423" t="n"/>
+      <c r="E35" s="343" t="n"/>
+      <c r="F35" s="343" t="n"/>
+      <c r="G35" s="343" t="n"/>
+      <c r="H35" s="424" t="n"/>
       <c r="I35" s="364">
         <f>(H35-$E$27)+$H$2</f>
         <v/>
@@ -7039,21 +6959,11 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D36" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E36" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G36" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H36" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D36" s="425" t="n"/>
+      <c r="E36" s="344" t="n"/>
+      <c r="F36" s="344" t="n"/>
+      <c r="G36" s="344" t="n"/>
+      <c r="H36" s="426" t="n"/>
       <c r="I36" s="365">
         <f>(H36-$E$27)+$H$2</f>
         <v/>
@@ -7108,21 +7018,11 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D37" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E37" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G37" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H37" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D37" s="425" t="n"/>
+      <c r="E37" s="344" t="n"/>
+      <c r="F37" s="344" t="n"/>
+      <c r="G37" s="344" t="n"/>
+      <c r="H37" s="426" t="n"/>
       <c r="I37" s="365">
         <f>(H37-$E$27)+$H$2</f>
         <v/>
@@ -7177,21 +7077,11 @@
         <f>SetPnt_P_3</f>
         <v/>
       </c>
-      <c r="D38" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E38" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G38" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H38" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D38" s="425" t="n"/>
+      <c r="E38" s="344" t="n"/>
+      <c r="F38" s="344" t="n"/>
+      <c r="G38" s="344" t="n"/>
+      <c r="H38" s="426" t="n"/>
       <c r="I38" s="365">
         <f>(H38-$E$27)+$H$2</f>
         <v/>
@@ -7246,21 +7136,11 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D39" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E39" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G39" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H39" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D39" s="425" t="n"/>
+      <c r="E39" s="344" t="n"/>
+      <c r="F39" s="344" t="n"/>
+      <c r="G39" s="344" t="n"/>
+      <c r="H39" s="426" t="n"/>
       <c r="I39" s="365">
         <f>(H39-$E$27)+$H$2</f>
         <v/>
@@ -7315,21 +7195,11 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D40" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E40" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G40" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H40" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D40" s="425" t="n"/>
+      <c r="E40" s="344" t="n"/>
+      <c r="F40" s="344" t="n"/>
+      <c r="G40" s="344" t="n"/>
+      <c r="H40" s="426" t="n"/>
       <c r="I40" s="365">
         <f>(H40-$E$27)+$H$2</f>
         <v/>
@@ -7384,21 +7254,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D41" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E41" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G41" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H41" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D41" s="423" t="n"/>
+      <c r="E41" s="343" t="n"/>
+      <c r="F41" s="343" t="n"/>
+      <c r="G41" s="343" t="n"/>
+      <c r="H41" s="424" t="n"/>
       <c r="I41" s="364">
         <f>(H41-$E$27)+$H$2</f>
         <v/>
@@ -7453,21 +7313,11 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D42" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E42" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G42" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H42" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D42" s="425" t="n"/>
+      <c r="E42" s="344" t="n"/>
+      <c r="F42" s="344" t="n"/>
+      <c r="G42" s="344" t="n"/>
+      <c r="H42" s="426" t="n"/>
       <c r="I42" s="365">
         <f>(H42-$E$27)+$H$2</f>
         <v/>
@@ -7522,21 +7372,11 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D43" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E43" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G43" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H43" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D43" s="425" t="n"/>
+      <c r="E43" s="344" t="n"/>
+      <c r="F43" s="344" t="n"/>
+      <c r="G43" s="344" t="n"/>
+      <c r="H43" s="426" t="n"/>
       <c r="I43" s="365">
         <f>(H43-$E$27)+$H$2</f>
         <v/>
@@ -7591,21 +7431,11 @@
         <f>SetPnt_P_3</f>
         <v/>
       </c>
-      <c r="D44" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E44" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G44" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H44" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D44" s="425" t="n"/>
+      <c r="E44" s="344" t="n"/>
+      <c r="F44" s="344" t="n"/>
+      <c r="G44" s="344" t="n"/>
+      <c r="H44" s="426" t="n"/>
       <c r="I44" s="365">
         <f>(H44-$E$27)+$H$2</f>
         <v/>
@@ -7660,21 +7490,11 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D45" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E45" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G45" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H45" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D45" s="425" t="n"/>
+      <c r="E45" s="344" t="n"/>
+      <c r="F45" s="344" t="n"/>
+      <c r="G45" s="344" t="n"/>
+      <c r="H45" s="426" t="n"/>
       <c r="I45" s="365">
         <f>(H45-$E$27)+$H$2</f>
         <v/>
@@ -7729,21 +7549,11 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D46" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E46" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G46" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H46" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D46" s="425" t="n"/>
+      <c r="E46" s="344" t="n"/>
+      <c r="F46" s="344" t="n"/>
+      <c r="G46" s="344" t="n"/>
+      <c r="H46" s="426" t="n"/>
       <c r="I46" s="366">
         <f>(H46-$E$27)+$H$2</f>
         <v/>
@@ -7798,21 +7608,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D47" s="429" t="n">
-        <v>837</v>
-      </c>
-      <c r="E47" s="430" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="430" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G47" s="430" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H47" s="431" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D47" s="429" t="n"/>
+      <c r="E47" s="430" t="n"/>
+      <c r="F47" s="430" t="n"/>
+      <c r="G47" s="430" t="n"/>
+      <c r="H47" s="431" t="n"/>
       <c r="I47" s="366">
         <f>(H47-$E$27)+$H$2</f>
         <v/>
@@ -8881,7 +8681,7 @@
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="25.88671875" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
@@ -10472,7 +10272,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="15.5546875" customWidth="1" min="1" max="1"/>
     <col width="19.6640625" customWidth="1" min="2" max="2"/>
@@ -16695,7 +16495,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="14.33203125" customWidth="1" min="1" max="1"/>
     <col width="19.6640625" customWidth="1" min="2" max="2"/>
@@ -22892,7 +22692,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col width="9" customWidth="1" min="2" max="2"/>
     <col width="13.5546875" customWidth="1" min="3" max="3"/>
@@ -24057,7 +23857,7 @@
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col width="3" customWidth="1" min="1" max="1"/>
     <col width="3.5546875" customWidth="1" min="2" max="2"/>
@@ -25566,8 +25366,8 @@
     <mergeCell ref="F16:M16"/>
     <mergeCell ref="G98:H98"/>
     <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G97:H97"/>
     <mergeCell ref="L102:L103"/>
-    <mergeCell ref="G97:H97"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="I91:J91"/>

</xml_diff>